<commit_message>
Add simple xslx file parsing
</commit_message>
<xml_diff>
--- a/docs/SurveyUpload.xlsx
+++ b/docs/SurveyUpload.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\repos\satoca\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288BCC4F-480F-4DFF-9EFA-10DC8D79A459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -53,7 +59,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -330,13 +336,131 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:A23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add management of multiple sheets
</commit_message>
<xml_diff>
--- a/docs/SurveyUpload.xlsx
+++ b/docs/SurveyUpload.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\repos\satoca\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{288BCC4F-480F-4DFF-9EFA-10DC8D79A459}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB86837-4B36-431B-86BC-D4D961F32E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
+    <sheet name="Survey" sheetId="1" r:id="rId1"/>
+    <sheet name="Options" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -337,130 +338,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846F55B4-4F48-439E-94FD-CA007324F3A3}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented the XLSX Parse into Database
</commit_message>
<xml_diff>
--- a/docs/SurveyUpload.xlsx
+++ b/docs/SurveyUpload.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\repos\satoca\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\WebstormProjects\SATOCA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB86837-4B36-431B-86BC-D4D961F32E9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1E958D-896C-4556-9CA8-80B368912126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -23,6 +23,59 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+  <si>
+    <t>Question</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Solution</t>
+  </si>
+  <si>
+    <t>Pizza?</t>
+  </si>
+  <si>
+    <t>Tomaten</t>
+  </si>
+  <si>
+    <t>Schinken</t>
+  </si>
+  <si>
+    <t>Käse</t>
+  </si>
+  <si>
+    <t>Salami</t>
+  </si>
+  <si>
+    <t>Ananas</t>
+  </si>
+  <si>
+    <t>Döner?</t>
+  </si>
+  <si>
+    <t>Scharf</t>
+  </si>
+  <si>
+    <t>Vegetarisch</t>
+  </si>
+  <si>
+    <t>Fleisch</t>
+  </si>
+  <si>
+    <t>1;2</t>
+  </si>
+  <si>
+    <t>Nudeln?</t>
+  </si>
+  <si>
+    <t>Sahne</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -338,14 +391,111 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="8" width="12.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1">
+        <v>1</v>
+      </c>
+      <c r="D1">
+        <v>2</v>
+      </c>
+      <c r="E1">
+        <v>3</v>
+      </c>
+      <c r="F1">
+        <v>4</v>
+      </c>
+      <c r="G1">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" t="s">
+        <v>12</v>
+      </c>
+      <c r="H3" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -354,7 +504,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846F55B4-4F48-439E-94FD-CA007324F3A3}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>

<commit_message>
Add Options processing for title and placeholder for other options
</commit_message>
<xml_diff>
--- a/docs/SurveyUpload.xlsx
+++ b/docs/SurveyUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Florian\WebstormProjects\SATOCA\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekte\satoca\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1E958D-896C-4556-9CA8-80B368912126}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90DBC0B-963F-466A-86CC-3C4C97D2E1BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
   <si>
     <t>Question</t>
   </si>
@@ -74,6 +74,15 @@
   </si>
   <si>
     <t>Sahne</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>Number participants</t>
+  </si>
+  <si>
+    <t>Super survey</t>
   </si>
 </sst>
 </file>
@@ -393,8 +402,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -502,12 +511,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846F55B4-4F48-439E-94FD-CA007324F3A3}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix survey and question/answer upload
</commit_message>
<xml_diff>
--- a/docs/SurveyUpload.xlsx
+++ b/docs/SurveyUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekte\satoca\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\repos\satoca\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E90DBC0B-963F-466A-86CC-3C4C97D2E1BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F1F116-6F32-487E-90E4-13AAB75EC635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4125" yWindow="825" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Question</t>
   </si>
@@ -83,16 +83,37 @@
   </si>
   <si>
     <t>Super survey</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -118,8 +139,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -402,7 +424,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
@@ -419,20 +441,20 @@
       <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="C1">
-        <v>1</v>
-      </c>
-      <c r="D1">
-        <v>2</v>
-      </c>
-      <c r="E1">
-        <v>3</v>
-      </c>
-      <c r="F1">
-        <v>4</v>
-      </c>
-      <c r="G1">
-        <v>5</v>
+      <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E1" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
       </c>
       <c r="H1" t="s">
         <v>2</v>
@@ -460,7 +482,7 @@
       <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="1">
         <v>3</v>
       </c>
     </row>
@@ -500,11 +522,12 @@
       <c r="D4" t="s">
         <v>15</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="1">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -513,7 +536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846F55B4-4F48-439E-94FD-CA007324F3A3}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Adjust Excel-Template and fileScheme in the backend
</commit_message>
<xml_diff>
--- a/docs/SurveyUpload.xlsx
+++ b/docs/SurveyUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\repos\satoca\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0F1F116-6F32-487E-90E4-13AAB75EC635}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5D0AF27-3260-479C-8299-28F2E911E267}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4125" yWindow="825" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
   <si>
     <t>Question</t>
   </si>
@@ -49,27 +49,12 @@
     <t>Käse</t>
   </si>
   <si>
-    <t>Salami</t>
-  </si>
-  <si>
-    <t>Ananas</t>
-  </si>
-  <si>
     <t>Döner?</t>
   </si>
   <si>
     <t>Scharf</t>
   </si>
   <si>
-    <t>Vegetarisch</t>
-  </si>
-  <si>
-    <t>Fleisch</t>
-  </si>
-  <si>
-    <t>1;2</t>
-  </si>
-  <si>
     <t>Nudeln?</t>
   </si>
   <si>
@@ -91,13 +76,16 @@
     <t>A2</t>
   </si>
   <si>
-    <t>A3</t>
-  </si>
-  <si>
-    <t>A4</t>
-  </si>
-  <si>
-    <t>A5</t>
+    <t>Difficulty</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>StartSet</t>
   </si>
 </sst>
 </file>
@@ -425,13 +413,15 @@
   <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="8" width="12.7109375" customWidth="1"/>
+    <col min="2" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -442,22 +432,22 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E1" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" t="s">
-        <v>21</v>
-      </c>
-      <c r="F1" t="s">
-        <v>22</v>
-      </c>
       <c r="G1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s">
-        <v>2</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -473,40 +463,32 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" t="s">
-        <v>6</v>
+      <c r="E2">
+        <v>3</v>
       </c>
       <c r="F2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="1">
-        <v>3</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="H2" s="1"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
-      <c r="E3" t="s">
-        <v>11</v>
+      <c r="E3">
+        <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="H3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -514,21 +496,23 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>4</v>
       </c>
       <c r="D4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4" s="1">
+        <v>10</v>
+      </c>
+      <c r="E4">
         <v>1</v>
       </c>
+      <c r="H4" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -548,15 +532,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B2">
         <v>16</v>

</xml_diff>

<commit_message>
Reformat excel template and add up to 5 answers
</commit_message>
<xml_diff>
--- a/docs/SurveyUpload.xlsx
+++ b/docs/SurveyUpload.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\repos\satoca\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EA930D6-F7DE-4584-ACD7-A690BEF3F0B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBF13CE-C99C-48FD-8151-FC80996F1192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Question</t>
   </si>
@@ -86,6 +86,15 @@
   </si>
   <si>
     <t>StartSet</t>
+  </si>
+  <si>
+    <t>A3</t>
+  </si>
+  <si>
+    <t>A4</t>
+  </si>
+  <si>
+    <t>A5</t>
   </si>
 </sst>
 </file>
@@ -127,9 +136,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -410,21 +420,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="12.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="12.7109375" customWidth="1"/>
+    <col min="2" max="3" width="12.7109375" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -432,82 +442,134 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G1" t="s">
-        <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>17</v>
+      <c r="I1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>1.2</v>
+      </c>
+      <c r="F2" s="2">
+        <v>10.1</v>
+      </c>
+      <c r="G2" t="s">
         <v>4</v>
       </c>
-      <c r="D2" t="s">
+      <c r="H2" t="s">
         <v>5</v>
       </c>
-      <c r="E2">
-        <v>2</v>
-      </c>
-      <c r="F2" t="s">
-        <v>18</v>
-      </c>
-      <c r="H2" s="1"/>
+      <c r="I2">
+        <v>3</v>
+      </c>
+      <c r="J2">
+        <v>4</v>
+      </c>
+      <c r="K2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>0.5</v>
+      </c>
+      <c r="F3" s="1">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
+      <c r="H3" t="s">
         <v>6</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
+      <c r="I3">
+        <v>3</v>
+      </c>
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3">
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F4" s="2">
+        <v>0.75</v>
+      </c>
+      <c r="G4" t="s">
         <v>4</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" t="s">
         <v>10</v>
       </c>
-      <c r="E4">
-        <v>2</v>
-      </c>
-      <c r="H4" s="1"/>
+      <c r="I4">
+        <v>3</v>
+      </c>
+      <c r="J4">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
add minimal information gain to database - version 2
</commit_message>
<xml_diff>
--- a/docs/SurveyUpload.xlsx
+++ b/docs/SurveyUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\repos\satoca\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\SATOCA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFBF13CE-C99C-48FD-8151-FC80996F1192}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A81539D-BB3A-44DF-98C0-021D1B6090D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Question</t>
   </si>
@@ -95,6 +95,9 @@
   </si>
   <si>
     <t>A5</t>
+  </si>
+  <si>
+    <t>Minimal information gain</t>
   </si>
 </sst>
 </file>
@@ -422,7 +425,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
@@ -580,10 +583,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846F55B4-4F48-439E-94FD-CA007324F3A3}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -608,6 +611,14 @@
         <v>16</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Add MinimalInformationGain to stop logic and make stop logic usable
</commit_message>
<xml_diff>
--- a/docs/SurveyUpload.xlsx
+++ b/docs/SurveyUpload.xlsx
@@ -5,21 +5,30 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\SATOCA\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\repos\satoca\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A81539D-BB3A-44DF-98C0-021D1B6090D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E84E0D-BA43-4502-AD0A-B584C35C70E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
     <sheet name="Options" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -426,7 +435,7 @@
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -586,7 +595,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,7 +625,7 @@
         <v>23</v>
       </c>
       <c r="B3">
-        <v>10</v>
+        <v>0.05</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Rename MinimalInformationGain to ItemSeverityBoundary
</commit_message>
<xml_diff>
--- a/docs/SurveyUpload.xlsx
+++ b/docs/SurveyUpload.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\repos\satoca\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73E84E0D-BA43-4502-AD0A-B584C35C70E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC065D8B-936E-4876-B0FD-059BD5F11824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1515" yWindow="1515" windowWidth="21600" windowHeight="11385" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -106,7 +106,7 @@
     <t>A5</t>
   </si>
   <si>
-    <t>Minimal information gain</t>
+    <t>Item severity boundary</t>
   </si>
 </sst>
 </file>
@@ -595,12 +595,12 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
add privacy budget to survey
</commit_message>
<xml_diff>
--- a/docs/SurveyUpload.xlsx
+++ b/docs/SurveyUpload.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\projects\repos\satoca\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\SATOCA\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC065D8B-936E-4876-B0FD-059BD5F11824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FEED08E-8193-485C-B651-0BDDBDC42BA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Survey" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Question</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>Item severity boundary</t>
+  </si>
+  <si>
+    <t>Privacy Budget</t>
   </si>
 </sst>
 </file>
@@ -592,10 +595,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{846F55B4-4F48-439E-94FD-CA007324F3A3}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -628,6 +631,14 @@
         <v>0.05</v>
       </c>
     </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4">
+        <v>0.8</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>